<commit_message>
evaluation data fixed, evaluation data added, bugs fixed, functionality added to save uncertaintypropagation model
</commit_message>
<xml_diff>
--- a/EvaluationData/Q3.2_Relevance.xlsx
+++ b/EvaluationData/Q3.2_Relevance.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Desktop\Masterarbeit\UncertaintyImpactAnalysis\EvaluationData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B655B25F-2F37-42BB-9C28-5AD4049A8470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBEA02D-A537-47D5-903A-9E733BD32C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="330" yWindow="1365" windowWidth="21600" windowHeight="12990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="96">
   <si>
     <t>ID</t>
   </si>
@@ -310,13 +319,16 @@
   </si>
   <si>
     <t xml:space="preserve"> -&gt; 21 Classes</t>
+  </si>
+  <si>
+    <t>See Uncertainty_Template_CWA.xlsx for categorisation to derive equivalence classes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,6 +346,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -365,11 +384,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -379,6 +395,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -659,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U32"/>
+  <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,80 +708,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="K1" s="1" t="s">
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="K1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="R1" s="1" t="s">
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="R1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-    </row>
-    <row r="2" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+    </row>
+    <row r="2" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="5" t="s">
+      <c r="K2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -769,14 +789,14 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="2"/>
       <c r="F3" t="s">
         <v>72</v>
       </c>
@@ -786,7 +806,7 @@
       <c r="H3" t="s">
         <v>84</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="5">
         <v>1</v>
       </c>
       <c r="K3" t="s">
@@ -824,14 +844,14 @@
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2"/>
       <c r="F4" t="s">
         <v>69</v>
       </c>
@@ -841,7 +861,7 @@
       <c r="H4" t="s">
         <v>84</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>2</v>
       </c>
       <c r="K4" t="s">
@@ -879,14 +899,14 @@
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
         <v>3</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="2"/>
       <c r="F5" t="s">
         <v>69</v>
       </c>
@@ -896,7 +916,7 @@
       <c r="H5" t="s">
         <v>84</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>2</v>
       </c>
       <c r="K5" t="s">
@@ -934,14 +954,14 @@
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3">
-        <v>2</v>
-      </c>
-      <c r="E6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2"/>
       <c r="F6" t="s">
         <v>69</v>
       </c>
@@ -951,7 +971,7 @@
       <c r="H6" t="s">
         <v>84</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <v>2</v>
       </c>
       <c r="K6" t="s">
@@ -989,14 +1009,14 @@
       <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="3">
+      <c r="C7" s="3"/>
+      <c r="D7" s="2">
         <v>4</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="3"/>
       <c r="F7" t="s">
         <v>69</v>
       </c>
@@ -1006,7 +1026,7 @@
       <c r="H7" t="s">
         <v>84</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <v>2</v>
       </c>
       <c r="K7" t="s">
@@ -1044,14 +1064,14 @@
       <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2">
         <v>5</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="2"/>
       <c r="F8" t="s">
         <v>71</v>
       </c>
@@ -1061,7 +1081,7 @@
       <c r="H8" t="s">
         <v>84</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>3</v>
       </c>
       <c r="K8" t="s">
@@ -1099,14 +1119,14 @@
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2">
         <v>6</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="2"/>
       <c r="F9" t="s">
         <v>69</v>
       </c>
@@ -1116,7 +1136,7 @@
       <c r="H9" t="s">
         <v>84</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <v>2</v>
       </c>
       <c r="K9" t="s">
@@ -1154,14 +1174,14 @@
       <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2">
         <v>7</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="2"/>
       <c r="F10" t="s">
         <v>72</v>
       </c>
@@ -1171,7 +1191,7 @@
       <c r="H10" t="s">
         <v>84</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="5">
         <v>1</v>
       </c>
       <c r="K10" t="s">
@@ -1209,14 +1229,14 @@
       <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2">
         <v>8</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="2"/>
       <c r="F11" t="s">
         <v>69</v>
       </c>
@@ -1226,7 +1246,7 @@
       <c r="H11" t="s">
         <v>84</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="5">
         <v>2</v>
       </c>
       <c r="K11" t="s">
@@ -1264,14 +1284,14 @@
       <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
         <v>9</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="2"/>
       <c r="F12" t="s">
         <v>69</v>
       </c>
@@ -1281,7 +1301,7 @@
       <c r="H12" t="s">
         <v>84</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="5">
         <v>2</v>
       </c>
       <c r="K12" t="s">
@@ -1319,14 +1339,14 @@
       <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
         <v>6</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="2"/>
       <c r="F13" t="s">
         <v>69</v>
       </c>
@@ -1336,7 +1356,7 @@
       <c r="H13" t="s">
         <v>84</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="5">
         <v>2</v>
       </c>
       <c r="K13" t="s">
@@ -1374,14 +1394,14 @@
       <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2">
         <v>10</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="2"/>
       <c r="F14" t="s">
         <v>72</v>
       </c>
@@ -1391,7 +1411,7 @@
       <c r="H14" t="s">
         <v>84</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="5">
         <v>1</v>
       </c>
       <c r="K14" t="s">
@@ -1429,14 +1449,14 @@
       <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2">
         <v>11</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="2"/>
       <c r="F15" t="s">
         <v>69</v>
       </c>
@@ -1446,7 +1466,7 @@
       <c r="H15" t="s">
         <v>84</v>
       </c>
-      <c r="I15" s="6">
+      <c r="I15" s="5">
         <v>2</v>
       </c>
       <c r="K15" t="s">
@@ -1484,14 +1504,14 @@
       <c r="A16" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="3">
+      <c r="C16" s="3"/>
+      <c r="D16" s="2">
         <v>12</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="3"/>
       <c r="F16" t="s">
         <v>69</v>
       </c>
@@ -1501,7 +1521,7 @@
       <c r="H16" t="s">
         <v>84</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="5">
         <v>2</v>
       </c>
       <c r="K16" t="s">
@@ -1539,14 +1559,14 @@
       <c r="A17" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2">
         <v>13</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="2"/>
       <c r="F17" t="s">
         <v>69</v>
       </c>
@@ -1556,7 +1576,7 @@
       <c r="H17" t="s">
         <v>84</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="5">
         <v>2</v>
       </c>
       <c r="K17" t="s">
@@ -1594,14 +1614,14 @@
       <c r="A18" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2">
         <v>6</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="2"/>
       <c r="F18" t="s">
         <v>69</v>
       </c>
@@ -1611,7 +1631,7 @@
       <c r="H18" t="s">
         <v>84</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="5">
         <v>2</v>
       </c>
       <c r="K18" t="s">
@@ -1649,14 +1669,14 @@
       <c r="A19" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2">
         <v>14</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="2"/>
       <c r="F19" t="s">
         <v>72</v>
       </c>
@@ -1666,7 +1686,7 @@
       <c r="H19" t="s">
         <v>84</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="5">
         <v>1</v>
       </c>
       <c r="K19" t="s">
@@ -1704,14 +1724,14 @@
       <c r="A20" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2">
         <v>1</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="2"/>
       <c r="F20" t="s">
         <v>72</v>
       </c>
@@ -1721,7 +1741,7 @@
       <c r="H20" t="s">
         <v>84</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="5">
         <v>1</v>
       </c>
       <c r="K20" t="s">
@@ -1759,14 +1779,14 @@
       <c r="A21" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2">
         <v>8</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="2"/>
       <c r="F21" t="s">
         <v>71</v>
       </c>
@@ -1776,7 +1796,7 @@
       <c r="H21" t="s">
         <v>84</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="5">
         <v>3</v>
       </c>
       <c r="K21" t="s">
@@ -1814,14 +1834,14 @@
       <c r="A22" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2">
         <v>3</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="2"/>
       <c r="F22" t="s">
         <v>69</v>
       </c>
@@ -1831,7 +1851,7 @@
       <c r="H22" t="s">
         <v>84</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="5">
         <v>2</v>
       </c>
       <c r="K22" t="s">
@@ -1869,14 +1889,14 @@
       <c r="A23" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2">
         <v>15</v>
       </c>
-      <c r="E23" s="3"/>
+      <c r="E23" s="2"/>
       <c r="F23" t="s">
         <v>69</v>
       </c>
@@ -1886,7 +1906,7 @@
       <c r="H23" t="s">
         <v>84</v>
       </c>
-      <c r="I23" s="6">
+      <c r="I23" s="5">
         <v>2</v>
       </c>
       <c r="K23" t="s">
@@ -1924,14 +1944,14 @@
       <c r="A24" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3">
-        <v>2</v>
-      </c>
-      <c r="E24" s="3"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2">
+        <v>2</v>
+      </c>
+      <c r="E24" s="2"/>
       <c r="F24" t="s">
         <v>69</v>
       </c>
@@ -1941,7 +1961,7 @@
       <c r="H24" t="s">
         <v>84</v>
       </c>
-      <c r="I24" s="6">
+      <c r="I24" s="5">
         <v>2</v>
       </c>
       <c r="K24" t="s">
@@ -1979,14 +1999,14 @@
       <c r="A25" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2">
         <v>16</v>
       </c>
-      <c r="E25" s="3"/>
+      <c r="E25" s="2"/>
       <c r="F25" t="s">
         <v>69</v>
       </c>
@@ -1996,7 +2016,7 @@
       <c r="H25" t="s">
         <v>84</v>
       </c>
-      <c r="I25" s="6">
+      <c r="I25" s="5">
         <v>2</v>
       </c>
       <c r="K25" t="s">
@@ -2034,14 +2054,14 @@
       <c r="A26" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2">
         <v>17</v>
       </c>
-      <c r="E26" s="3"/>
+      <c r="E26" s="2"/>
       <c r="F26" t="s">
         <v>69</v>
       </c>
@@ -2051,7 +2071,7 @@
       <c r="H26" t="s">
         <v>84</v>
       </c>
-      <c r="I26" s="6">
+      <c r="I26" s="5">
         <v>2</v>
       </c>
       <c r="K26" t="s">
@@ -2089,14 +2109,14 @@
       <c r="A27" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2">
         <v>18</v>
       </c>
-      <c r="E27" s="3"/>
+      <c r="E27" s="2"/>
       <c r="F27" t="s">
         <v>69</v>
       </c>
@@ -2106,7 +2126,7 @@
       <c r="H27" t="s">
         <v>84</v>
       </c>
-      <c r="I27" s="6">
+      <c r="I27" s="5">
         <v>2</v>
       </c>
       <c r="K27" t="s">
@@ -2144,14 +2164,14 @@
       <c r="A28" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3">
+      <c r="C28" s="2"/>
+      <c r="D28" s="2">
         <v>19</v>
       </c>
-      <c r="E28" s="3"/>
+      <c r="E28" s="2"/>
       <c r="F28" t="s">
         <v>69</v>
       </c>
@@ -2161,7 +2181,7 @@
       <c r="H28" t="s">
         <v>84</v>
       </c>
-      <c r="I28" s="6">
+      <c r="I28" s="5">
         <v>2</v>
       </c>
       <c r="K28" t="s">
@@ -2199,14 +2219,14 @@
       <c r="A29" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2">
         <v>20</v>
       </c>
-      <c r="E29" s="3"/>
+      <c r="E29" s="2"/>
       <c r="F29" t="s">
         <v>69</v>
       </c>
@@ -2216,7 +2236,7 @@
       <c r="H29" t="s">
         <v>84</v>
       </c>
-      <c r="I29" s="6">
+      <c r="I29" s="5">
         <v>2</v>
       </c>
       <c r="K29" t="s">
@@ -2254,14 +2274,14 @@
       <c r="A30" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2">
         <v>21</v>
       </c>
-      <c r="E30" s="3"/>
+      <c r="E30" s="2"/>
       <c r="F30" t="s">
         <v>71</v>
       </c>
@@ -2271,7 +2291,7 @@
       <c r="H30" t="s">
         <v>84</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I30" s="5">
         <v>3</v>
       </c>
       <c r="K30" t="s">
@@ -2317,6 +2337,11 @@
       </c>
       <c r="U32" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="6" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>